<commit_message>
Adjust membership function of blink rate
Now blink rate and its membership value are equivalent.
</commit_message>
<xml_diff>
--- a/fuzzy_grades.xlsx
+++ b/fuzzy_grades.xlsx
@@ -2728,7 +2728,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2738,64 +2738,70 @@
   <sheetData>
     <row r="1">
       <c r="B1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="n">
+      <c r="E1" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="n">
+      <c r="F1" t="n">
         <v>4</v>
       </c>
-      <c r="F1" t="n">
+      <c r="G1" t="n">
         <v>5</v>
       </c>
-      <c r="G1" t="n">
+      <c r="H1" t="n">
         <v>6</v>
       </c>
-      <c r="H1" t="n">
+      <c r="I1" t="n">
         <v>7</v>
       </c>
-      <c r="I1" t="n">
+      <c r="J1" t="n">
         <v>8</v>
       </c>
-      <c r="J1" t="n">
+      <c r="K1" t="n">
         <v>9</v>
       </c>
-      <c r="K1" t="n">
+      <c r="L1" t="n">
         <v>10</v>
       </c>
-      <c r="L1" t="n">
+      <c r="M1" t="n">
         <v>11</v>
       </c>
-      <c r="M1" t="n">
+      <c r="N1" t="n">
         <v>12</v>
       </c>
-      <c r="N1" t="n">
+      <c r="O1" t="n">
         <v>13</v>
       </c>
-      <c r="O1" t="n">
+      <c r="P1" t="n">
         <v>14</v>
       </c>
-      <c r="P1" t="n">
+      <c r="Q1" t="n">
         <v>15</v>
       </c>
-      <c r="Q1" t="n">
+      <c r="R1" t="n">
         <v>16</v>
       </c>
-      <c r="R1" t="n">
+      <c r="S1" t="n">
         <v>17</v>
       </c>
-      <c r="S1" t="n">
+      <c r="T1" t="n">
         <v>18</v>
       </c>
-      <c r="T1" t="n">
+      <c r="U1" t="n">
         <v>19</v>
       </c>
-      <c r="U1" t="n">
+      <c r="V1" t="n">
         <v>20</v>
+      </c>
+      <c r="W1" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -2803,64 +2809,70 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.09</v>
+        <v>0.59</v>
       </c>
       <c r="C2" t="n">
-        <v>0.18</v>
+        <v>0.59</v>
       </c>
       <c r="D2" t="n">
-        <v>0.27</v>
+        <v>0.59</v>
       </c>
       <c r="E2" t="n">
-        <v>0.36</v>
+        <v>0.59</v>
       </c>
       <c r="F2" t="n">
-        <v>0.42</v>
+        <v>0.59</v>
       </c>
       <c r="G2" t="n">
-        <v>0.42</v>
+        <v>0.59</v>
       </c>
       <c r="H2" t="n">
-        <v>0.42</v>
+        <v>0.59</v>
       </c>
       <c r="I2" t="n">
-        <v>0.42</v>
+        <v>0.59</v>
       </c>
       <c r="J2" t="n">
-        <v>0.42</v>
+        <v>0.59</v>
       </c>
       <c r="K2" t="n">
-        <v>0.42</v>
+        <v>0.55</v>
       </c>
       <c r="L2" t="n">
-        <v>0.42</v>
+        <v>0.52</v>
       </c>
       <c r="M2" t="n">
-        <v>0.42</v>
+        <v>0.47</v>
       </c>
       <c r="N2" t="n">
         <v>0.42</v>
       </c>
       <c r="O2" t="n">
-        <v>0.42</v>
+        <v>0.37</v>
       </c>
       <c r="P2" t="n">
-        <v>0.42</v>
+        <v>0.33</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="R2" t="n">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
       <c r="S2" t="n">
-        <v>0.18</v>
+        <v>0.26</v>
       </c>
       <c r="T2" t="n">
-        <v>0.09</v>
+        <v>0.24</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="W2" t="n">
+        <v>-0</v>
       </c>
     </row>
     <row r="3">
@@ -2868,64 +2880,70 @@
         <v>0.1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.11</v>
+        <v>0.6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.19</v>
+        <v>0.6</v>
       </c>
       <c r="D3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0.29</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.38</v>
       </c>
       <c r="R3" t="n">
         <v>0.29</v>
       </c>
       <c r="S3" t="n">
-        <v>0.19</v>
+        <v>0.27</v>
       </c>
       <c r="T3" t="n">
-        <v>0.11</v>
+        <v>0.25</v>
       </c>
       <c r="U3" t="n">
-        <v>0.01</v>
+        <v>0.21</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W3" t="n">
+        <v>-0</v>
       </c>
     </row>
     <row r="4">
@@ -2933,64 +2951,70 @@
         <v>0.2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.14</v>
+        <v>0.64</v>
       </c>
       <c r="C4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="U4" t="n">
         <v>0.23</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.05</v>
+      <c r="V4" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W4" t="n">
+        <v>-0</v>
       </c>
     </row>
     <row r="5">
@@ -2998,64 +3022,70 @@
         <v>0.3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.21</v>
+        <v>0.71</v>
       </c>
       <c r="C5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="T5" t="n">
         <v>0.31</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.21</v>
-      </c>
       <c r="U5" t="n">
-        <v>0.11</v>
+        <v>0.23</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W5" t="n">
+        <v>-0</v>
       </c>
     </row>
     <row r="6">
@@ -3063,64 +3093,70 @@
         <v>0.4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.26</v>
+        <v>0.82</v>
       </c>
       <c r="C6" t="n">
-        <v>0.36</v>
+        <v>0.82</v>
       </c>
       <c r="D6" t="n">
-        <v>0.44</v>
+        <v>0.82</v>
       </c>
       <c r="E6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="O6" t="n">
         <v>0.5</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.54</v>
-      </c>
       <c r="P6" t="n">
-        <v>0.54</v>
+        <v>0.45</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R6" t="n">
-        <v>0.44</v>
+        <v>0.39</v>
       </c>
       <c r="S6" t="n">
         <v>0.36</v>
       </c>
       <c r="T6" t="n">
-        <v>0.26</v>
+        <v>0.31</v>
       </c>
       <c r="U6" t="n">
-        <v>0.16</v>
+        <v>0.23</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W6" t="n">
+        <v>-0</v>
       </c>
     </row>
     <row r="7">
@@ -3128,64 +3164,70 @@
         <v>0.5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.29</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.51</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="L7" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="M7" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="N7" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.58</v>
       </c>
       <c r="O7" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="P7" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.51</v>
+        <v>0.41</v>
       </c>
       <c r="R7" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="S7" t="n">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="T7" t="n">
-        <v>0.29</v>
+        <v>0.31</v>
       </c>
       <c r="U7" t="n">
-        <v>0.18</v>
+        <v>0.23</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W7" t="n">
+        <v>-0</v>
       </c>
     </row>
     <row r="8">
@@ -3193,64 +3235,70 @@
         <v>0.6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.29</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.46</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="O8" t="n">
         <v>0.52</v>
       </c>
-      <c r="F8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.5600000000000001</v>
-      </c>
       <c r="P8" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.52</v>
+        <v>0.49</v>
       </c>
       <c r="R8" t="n">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="S8" t="n">
-        <v>0.38</v>
+        <v>0.44</v>
       </c>
       <c r="T8" t="n">
-        <v>0.29</v>
+        <v>0.4</v>
       </c>
       <c r="U8" t="n">
-        <v>0.29</v>
+        <v>0.34</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="9">
@@ -3258,64 +3306,70 @@
         <v>0.7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0.39</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.48</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.54</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.58</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.58</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0.58</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.58</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.58</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.58</v>
+        <v>0.84</v>
       </c>
       <c r="L9" t="n">
-        <v>0.58</v>
+        <v>0.73</v>
       </c>
       <c r="M9" t="n">
-        <v>0.58</v>
+        <v>0.65</v>
       </c>
       <c r="N9" t="n">
         <v>0.58</v>
       </c>
       <c r="O9" t="n">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="P9" t="n">
-        <v>0.58</v>
+        <v>0.55</v>
       </c>
       <c r="Q9" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="R9" t="n">
         <v>0.54</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="T9" t="n">
         <v>0.48</v>
       </c>
-      <c r="S9" t="n">
+      <c r="U9" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="W9" t="n">
         <v>0.39</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0.38</v>
       </c>
     </row>
     <row r="10">
@@ -3323,64 +3377,70 @@
         <v>0.8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.46</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="W10" t="n">
         <v>0.48</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="T10" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0.45</v>
       </c>
     </row>
     <row r="11">
@@ -3388,64 +3448,70 @@
         <v>0.9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.52</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>0.54</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.59</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>0.75</v>
+        <v>0.84</v>
       </c>
       <c r="L11" t="n">
         <v>0.75</v>
       </c>
       <c r="M11" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="N11" t="n">
-        <v>0.75</v>
+        <v>0.67</v>
       </c>
       <c r="O11" t="n">
-        <v>0.75</v>
+        <v>0.66</v>
       </c>
       <c r="P11" t="n">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="R11" t="n">
-        <v>0.59</v>
+        <v>0.64</v>
       </c>
       <c r="S11" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="W11" t="n">
         <v>0.54</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0.51</v>
       </c>
     </row>
     <row r="12">
@@ -3453,64 +3519,70 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.58</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="T12" t="n">
         <v>0.64</v>
       </c>
-      <c r="E12" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" t="n">
-        <v>1</v>
-      </c>
-      <c r="P12" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0.5600000000000001</v>
-      </c>
       <c r="U12" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.61</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify range of contour chart and add comments
</commit_message>
<xml_diff>
--- a/fuzzy_grades.xlsx
+++ b/fuzzy_grades.xlsx
@@ -633,6 +633,54 @@
             </numRef>
           </val>
         </ser>
+        <ser>
+          <idx val="20"/>
+          <order val="20"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!V1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$V$2:$V$12</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="21"/>
+          <order val="21"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!W1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$W$2:$W$12</f>
+            </numRef>
+          </val>
+        </ser>
         <axId val="10"/>
         <axId val="100"/>
         <axId val="1000"/>
@@ -1190,6 +1238,54 @@
             </numRef>
           </val>
         </ser>
+        <ser>
+          <idx val="20"/>
+          <order val="20"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!V1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$V$2:$V$12</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="21"/>
+          <order val="21"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!W1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$W$2:$W$12</f>
+            </numRef>
+          </val>
+        </ser>
         <axId val="10"/>
         <axId val="100"/>
         <axId val="1000"/>
@@ -1745,6 +1841,54 @@
             </numRef>
           </val>
         </ser>
+        <ser>
+          <idx val="20"/>
+          <order val="20"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!V1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$V$2:$V$12</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="21"/>
+          <order val="21"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!W1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$W$2:$W$12</f>
+            </numRef>
+          </val>
+        </ser>
         <axId val="10"/>
         <axId val="100"/>
         <axId val="1000"/>
@@ -2297,6 +2441,54 @@
           <val>
             <numRef>
               <f>'Sheet'!$U$2:$U$12</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="20"/>
+          <order val="20"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!V1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$V$2:$V$12</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="21"/>
+          <order val="21"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!W1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$W$2:$W$12</f>
             </numRef>
           </val>
         </ser>

</xml_diff>

<commit_message>
Add documentations of parse and chart
</commit_message>
<xml_diff>
--- a/fuzzy_grades.xlsx
+++ b/fuzzy_grades.xlsx
@@ -3064,7 +3064,7 @@
         <v>0.12</v>
       </c>
       <c r="W2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -3135,7 +3135,7 @@
         <v>0.13</v>
       </c>
       <c r="W3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -3206,7 +3206,7 @@
         <v>0.13</v>
       </c>
       <c r="W4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -3277,7 +3277,7 @@
         <v>0.13</v>
       </c>
       <c r="W5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -3348,7 +3348,7 @@
         <v>0.13</v>
       </c>
       <c r="W6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -3419,7 +3419,7 @@
         <v>0.13</v>
       </c>
       <c r="W7" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Make normalization of fuzzy grade optional
Also the fuzzy rule is adjusted since the 1.0 area has been over-large.
And some documentations added.
</commit_message>
<xml_diff>
--- a/fuzzy_grades.xlsx
+++ b/fuzzy_grades.xlsx
@@ -2929,6 +2929,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
       <c r="B1" t="n">
         <v>0</v>
       </c>
@@ -3132,10 +3135,10 @@
         <v>0.21</v>
       </c>
       <c r="V3" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="W3" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="4">
@@ -3143,37 +3146,37 @@
         <v>0.2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="C4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="D4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="E4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="F4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="G4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="H4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="I4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="J4" t="n">
-        <v>0.64</v>
+        <v>0.62</v>
       </c>
       <c r="K4" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="L4" t="n">
-        <v>0.57</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="M4" t="n">
         <v>0.52</v>
@@ -3200,13 +3203,13 @@
         <v>0.28</v>
       </c>
       <c r="U4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.23</v>
       </c>
-      <c r="V4" t="n">
-        <v>0.13</v>
-      </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="5">
@@ -3214,43 +3217,43 @@
         <v>0.3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="C5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="D5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="E5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="F5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="G5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="H5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="I5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="J5" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="K5" t="n">
-        <v>0.67</v>
+        <v>0.63</v>
       </c>
       <c r="L5" t="n">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
       <c r="M5" t="n">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="N5" t="n">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="O5" t="n">
         <v>0.46</v>
@@ -3268,16 +3271,16 @@
         <v>0.35</v>
       </c>
       <c r="T5" t="n">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="U5" t="n">
-        <v>0.23</v>
+        <v>0.28</v>
       </c>
       <c r="V5" t="n">
-        <v>0.13</v>
+        <v>0.26</v>
       </c>
       <c r="W5" t="n">
-        <v>0</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="6">
@@ -3285,43 +3288,43 @@
         <v>0.4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="C6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="D6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="E6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="F6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="G6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="H6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="I6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="J6" t="n">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="K6" t="n">
-        <v>0.78</v>
+        <v>0.65</v>
       </c>
       <c r="L6" t="n">
-        <v>0.71</v>
+        <v>0.63</v>
       </c>
       <c r="M6" t="n">
-        <v>0.63</v>
+        <v>0.59</v>
       </c>
       <c r="N6" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="O6" t="n">
         <v>0.5</v>
@@ -3336,19 +3339,19 @@
         <v>0.39</v>
       </c>
       <c r="S6" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="T6" t="n">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="U6" t="n">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="V6" t="n">
-        <v>0.13</v>
+        <v>0.28</v>
       </c>
       <c r="W6" t="n">
-        <v>0</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="7">
@@ -3356,43 +3359,43 @@
         <v>0.5</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="K7" t="n">
-        <v>0.84</v>
+        <v>0.66</v>
       </c>
       <c r="L7" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="M7" t="n">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="N7" t="n">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="O7" t="n">
         <v>0.52</v>
@@ -3407,19 +3410,19 @@
         <v>0.4</v>
       </c>
       <c r="S7" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="T7" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="U7" t="n">
         <v>0.31</v>
       </c>
-      <c r="U7" t="n">
-        <v>0.23</v>
-      </c>
       <c r="V7" t="n">
-        <v>0.13</v>
+        <v>0.29</v>
       </c>
       <c r="W7" t="n">
-        <v>0</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="8">
@@ -3427,43 +3430,43 @@
         <v>0.6</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="K8" t="n">
-        <v>0.84</v>
+        <v>0.67</v>
       </c>
       <c r="L8" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="M8" t="n">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="N8" t="n">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="O8" t="n">
         <v>0.52</v>
@@ -3478,19 +3481,19 @@
         <v>0.48</v>
       </c>
       <c r="S8" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="T8" t="n">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="U8" t="n">
-        <v>0.34</v>
+        <v>0.38</v>
       </c>
       <c r="V8" t="n">
-        <v>0.27</v>
+        <v>0.36</v>
       </c>
       <c r="W8" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="9">
@@ -3498,43 +3501,43 @@
         <v>0.7</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="K9" t="n">
-        <v>0.84</v>
+        <v>0.68</v>
       </c>
       <c r="L9" t="n">
-        <v>0.73</v>
+        <v>0.65</v>
       </c>
       <c r="M9" t="n">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="N9" t="n">
-        <v>0.58</v>
+        <v>0.57</v>
       </c>
       <c r="O9" t="n">
         <v>0.5600000000000001</v>
@@ -3558,10 +3561,10 @@
         <v>0.44</v>
       </c>
       <c r="V9" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="W9" t="n">
         <v>0.41</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0.39</v>
       </c>
     </row>
     <row r="10">
@@ -3569,37 +3572,37 @@
         <v>0.8</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="K10" t="n">
-        <v>0.84</v>
+        <v>0.72</v>
       </c>
       <c r="L10" t="n">
-        <v>0.73</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="M10" t="n">
         <v>0.65</v>
@@ -3640,34 +3643,34 @@
         <v>0.9</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="K11" t="n">
-        <v>0.84</v>
+        <v>0.8</v>
       </c>
       <c r="L11" t="n">
         <v>0.75</v>

</xml_diff>